<commit_message>
Parser now extracts course credits
</commit_message>
<xml_diff>
--- a/Schedulator/SoftwareAndCompCourseList.xlsx
+++ b/Schedulator/SoftwareAndCompCourseList.xlsx
@@ -19943,8 +19943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed courses to include if the course is an elective and what type
</commit_message>
<xml_diff>
--- a/Schedulator/SoftwareAndCompCourseList.xlsx
+++ b/Schedulator/SoftwareAndCompCourseList.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="COMPUTER SCIENCE" sheetId="1" r:id="rId1"/>
-    <sheet name="COOP WORK TERM (COMP SCI)" sheetId="2" r:id="rId2"/>
-    <sheet name="COOP WORK TERM (ENGINEERING)" sheetId="3" r:id="rId3"/>
-    <sheet name="ELECT. ENGINEERING" sheetId="4" r:id="rId4"/>
-    <sheet name="ENGING. COMP SCI" sheetId="5" r:id="rId5"/>
-    <sheet name="ENGINEERING" sheetId="6" r:id="rId6"/>
-    <sheet name="SOFTWARE ENGINEERING" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
+    <sheet name="COOP WORK TERM (COMP SCI)" sheetId="2" r:id="rId3"/>
+    <sheet name="COOP WORK TERM (ENGINEERING)" sheetId="3" r:id="rId4"/>
+    <sheet name="ELECT. ENGINEERING" sheetId="4" r:id="rId5"/>
+    <sheet name="ENGING. COMP SCI" sheetId="5" r:id="rId6"/>
+    <sheet name="ENGINEERING" sheetId="6" r:id="rId7"/>
+    <sheet name="SOFTWARE ENGINEERING" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5010" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5078" uniqueCount="1159">
   <si>
     <t>COMP 107</t>
   </si>
@@ -3489,19 +3490,46 @@
   </si>
   <si>
     <t>Students who have received credit for ENGR 275 may not take this course for credit. Students in Electrical Engineering or in Computer Engineering are not permitted to take this course.</t>
+  </si>
+  <si>
+    <t>MECH 221</t>
+  </si>
+  <si>
+    <t>MATERIALS SCIENCE</t>
+  </si>
+  <si>
+    <t>CHEM 205 (CEGEP Chemistry 101).</t>
+  </si>
+  <si>
+    <t>SGW MB-5.265</t>
+  </si>
+  <si>
+    <t>ABOU ZIKI, JANA</t>
+  </si>
+  <si>
+    <t>NOFAR, MOHAMMADREZA</t>
+  </si>
+  <si>
+    <t>Tut XB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3524,8 +3552,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3836,8 +3866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E437"/>
   <sheetViews>
-    <sheetView topLeftCell="A369" workbookViewId="0">
-      <selection activeCell="A436" sqref="A436"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9207,6 +9237,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
@@ -10021,11 +10063,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -11448,7 +11490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
@@ -12468,12 +12510,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13541,12 +13583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E476"/>
+  <dimension ref="A1:E494"/>
   <sheetViews>
-    <sheetView topLeftCell="A463" workbookViewId="0">
-      <selection activeCell="B469" sqref="B469"/>
+    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
+      <selection activeCell="B485" sqref="B485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19934,17 +19976,259 @@
         <v>687</v>
       </c>
     </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B477" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E477" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>17</v>
+      </c>
+      <c r="B478" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>14</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C480" t="s">
+        <v>185</v>
+      </c>
+      <c r="D480" t="s">
+        <v>165</v>
+      </c>
+      <c r="E480" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>25</v>
+      </c>
+      <c r="B481" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C481" t="s">
+        <v>552</v>
+      </c>
+      <c r="D481" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>14</v>
+      </c>
+      <c r="B482" s="2" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C482" t="s">
+        <v>552</v>
+      </c>
+      <c r="D482" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>14</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C483" t="s">
+        <v>185</v>
+      </c>
+      <c r="D483" t="s">
+        <v>573</v>
+      </c>
+      <c r="E483" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>14</v>
+      </c>
+      <c r="B484" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C484" t="s">
+        <v>552</v>
+      </c>
+      <c r="D484" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>14</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C485" t="s">
+        <v>552</v>
+      </c>
+      <c r="D485" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>14</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="C486" t="s">
+        <v>234</v>
+      </c>
+      <c r="D486" t="s">
+        <v>627</v>
+      </c>
+      <c r="E486" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>14</v>
+      </c>
+      <c r="B487" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C487" t="s">
+        <v>552</v>
+      </c>
+      <c r="D487" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>14</v>
+      </c>
+      <c r="B488" s="2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C488" t="s">
+        <v>552</v>
+      </c>
+      <c r="D488" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>29</v>
+      </c>
+      <c r="B489" s="1"/>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>30</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C490" t="s">
+        <v>185</v>
+      </c>
+      <c r="D490" t="s">
+        <v>96</v>
+      </c>
+      <c r="E490" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>30</v>
+      </c>
+      <c r="B491" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C491" t="s">
+        <v>552</v>
+      </c>
+      <c r="D491" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>30</v>
+      </c>
+      <c r="B492" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C492" t="s">
+        <v>552</v>
+      </c>
+      <c r="D492" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>30</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C493" t="s">
+        <v>185</v>
+      </c>
+      <c r="D493" t="s">
+        <v>235</v>
+      </c>
+      <c r="E493" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>30</v>
+      </c>
+      <c r="B494" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C494" t="s">
+        <v>552</v>
+      </c>
+      <c r="D494" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed missingprequs function bug
</commit_message>
<xml_diff>
--- a/Schedulator/SoftwareAndCompCourseList.xlsx
+++ b/Schedulator/SoftwareAndCompCourseList.xlsx
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5078" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5225" uniqueCount="1197">
   <si>
     <t>COMP 107</t>
   </si>
@@ -3511,6 +3511,120 @@
   </si>
   <si>
     <t>Tut XB</t>
+  </si>
+  <si>
+    <t>AERO 417</t>
+  </si>
+  <si>
+    <t>STNDRDS/REGUL N/CERTIF N</t>
+  </si>
+  <si>
+    <t>Students who have received credit for ENGR 417 may not take this course for credit.</t>
+  </si>
+  <si>
+    <t>AERO 431</t>
+  </si>
+  <si>
+    <t>PRINCIPLES OF AEROELASTICITY</t>
+  </si>
+  <si>
+    <t>ENGR 243, 311.</t>
+  </si>
+  <si>
+    <t>Students who have received credit for MECH 431 may not take this course for credit</t>
+  </si>
+  <si>
+    <t>AERO 462</t>
+  </si>
+  <si>
+    <t>TURBOMACHINERY+PROPULSION</t>
+  </si>
+  <si>
+    <t>MECH 351, 361</t>
+  </si>
+  <si>
+    <t>Students who have received credit for MECH 462may not take this course for credit</t>
+  </si>
+  <si>
+    <t>AERO 464</t>
+  </si>
+  <si>
+    <t>AERODYNAMICS</t>
+  </si>
+  <si>
+    <t>MECH 361</t>
+  </si>
+  <si>
+    <t>Student who have received credit for MECH 464 may not take this course for credit</t>
+  </si>
+  <si>
+    <t>AERO 465</t>
+  </si>
+  <si>
+    <t>GAS TURBINE DESIGN</t>
+  </si>
+  <si>
+    <t>Students who received credit for MECH 465 may not take this course for credit.</t>
+  </si>
+  <si>
+    <t>GIRGIS, SAMI</t>
+  </si>
+  <si>
+    <t>AERO 480</t>
+  </si>
+  <si>
+    <t>FLIGHT CONTROL SYSTEMS</t>
+  </si>
+  <si>
+    <t>AERO 371 or ELEC 372 or MECH 371 or SOEN 385</t>
+  </si>
+  <si>
+    <t>Students who received credit for ELEC 415 or MECH 480 may not take this course for credit.</t>
+  </si>
+  <si>
+    <t>M------ (11:45-13:35) Week(1)</t>
+  </si>
+  <si>
+    <t>SGW H-0011</t>
+  </si>
+  <si>
+    <t>M------ (11:45-13:35) Week(2)</t>
+  </si>
+  <si>
+    <t>--W---- (12:05-13:55) Week(1)</t>
+  </si>
+  <si>
+    <t>--W---- (12:05-13:55) Week(2)</t>
+  </si>
+  <si>
+    <t>--W---- (09:45-11:35) Week(1)</t>
+  </si>
+  <si>
+    <t>--W---- (09:45-11:35) Week(2)</t>
+  </si>
+  <si>
+    <t>--W---- (14:45-16:35) Week(1)</t>
+  </si>
+  <si>
+    <t>Lab XO</t>
+  </si>
+  <si>
+    <t>COEN 320</t>
+  </si>
+  <si>
+    <t>INTRO TO REAL-TIME SYSTEMS</t>
+  </si>
+  <si>
+    <t>COEN 346 or COMP 346.</t>
+  </si>
+  <si>
+    <t>--W---- (14:45-15:35)</t>
+  </si>
+  <si>
+    <t>SGW H-863</t>
+  </si>
+  <si>
+    <t>Tut SA</t>
   </si>
 </sst>
 </file>
@@ -13585,10 +13699,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E494"/>
+  <dimension ref="A1:E542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="B485" sqref="B485"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="E499" sqref="E499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20217,6 +20331,546 @@
         <v>63</v>
       </c>
     </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E495" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>19</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>14</v>
+      </c>
+      <c r="B498" t="s">
+        <v>996</v>
+      </c>
+      <c r="C498" t="s">
+        <v>177</v>
+      </c>
+      <c r="D498" t="s">
+        <v>670</v>
+      </c>
+      <c r="E498" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B499" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E499" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>17</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>19</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>14</v>
+      </c>
+      <c r="B503" t="s">
+        <v>332</v>
+      </c>
+      <c r="C503" t="s">
+        <v>95</v>
+      </c>
+      <c r="D503" t="s">
+        <v>230</v>
+      </c>
+      <c r="E503" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="504" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E504" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>17</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="506" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>19</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>14</v>
+      </c>
+      <c r="B508" t="s">
+        <v>996</v>
+      </c>
+      <c r="C508" t="s">
+        <v>22</v>
+      </c>
+      <c r="D508" t="s">
+        <v>758</v>
+      </c>
+      <c r="E508" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="509" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>25</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C509" t="s">
+        <v>27</v>
+      </c>
+      <c r="D509" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E510" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="511" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>17</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>19</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>29</v>
+      </c>
+      <c r="B513" s="1"/>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>30</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C514" t="s">
+        <v>22</v>
+      </c>
+      <c r="D514" t="s">
+        <v>670</v>
+      </c>
+      <c r="E514" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>33</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C515" t="s">
+        <v>27</v>
+      </c>
+      <c r="D515" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>33</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C516" t="s">
+        <v>27</v>
+      </c>
+      <c r="D516" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E517" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>17</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>19</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>29</v>
+      </c>
+      <c r="B520" s="1"/>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>30</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C521" t="s">
+        <v>121</v>
+      </c>
+      <c r="D521" t="s">
+        <v>104</v>
+      </c>
+      <c r="E521" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>33</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C522" t="s">
+        <v>7</v>
+      </c>
+      <c r="D522" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>33</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C523" t="s">
+        <v>7</v>
+      </c>
+      <c r="D523" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>33</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C524" t="s">
+        <v>7</v>
+      </c>
+      <c r="D524" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>33</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C525" t="s">
+        <v>7</v>
+      </c>
+      <c r="D525" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E526" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>17</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>19</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>13</v>
+      </c>
+      <c r="B529" s="1"/>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>14</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C530" t="s">
+        <v>121</v>
+      </c>
+      <c r="D530" t="s">
+        <v>117</v>
+      </c>
+      <c r="E530" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>25</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C531" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D531" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>25</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C532" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D532" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>25</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C533" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D533" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>25</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C534" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D534" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>25</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C535" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D535" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>25</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C536" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D536" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>25</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C537" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D537" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B538" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E538" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>17</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>14</v>
+      </c>
+      <c r="B541" t="s">
+        <v>112</v>
+      </c>
+      <c r="C541" t="s">
+        <v>262</v>
+      </c>
+      <c r="D541" t="s">
+        <v>641</v>
+      </c>
+      <c r="E541" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>14</v>
+      </c>
+      <c r="B542" s="2" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C542" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D542" t="s">
+        <v>1195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -20227,8 +20881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>